<commit_message>
first version deep learning template with pth file
</commit_message>
<xml_diff>
--- a/summary/summary.xlsx
+++ b/summary/summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -574,6 +574,53 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2022-11-16_20-48-47</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.9346306920051575</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>./checkpoints/2022-11-16_20-48-47</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>./record/2022-11-16_20-48-47</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>./log/2022-11-16_20-48-47</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>./log/2022-11-16_20-48-47/log.txt</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>